<commit_message>
Fixed all Dialog GUIs except Stage Related. Added Aux Classes
</commit_message>
<xml_diff>
--- a/Dataset/YACM-Dataset.xlsx
+++ b/Dataset/YACM-Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\UA\BD\Project\BD-YACM\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98328C04-0C5D-4E09-AE91-BA0E65B4A4D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E930C5-B564-4E74-8E66-6B7A984C67F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="4" xr2:uid="{67B48889-A8C9-4163-B416-5FF4F8CF7936}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{67B48889-A8C9-4163-B416-5FF4F8CF7936}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Participants @Events" sheetId="3" r:id="rId3"/>
     <sheet name="Sponsorhips and Prizes" sheetId="4" r:id="rId4"/>
     <sheet name="Stages" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="712">
   <si>
     <t>Nicholas Mason</t>
   </si>
@@ -2144,6 +2145,33 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>DOCUMENT</t>
+  </si>
+  <si>
+    <t>OTHERFILE</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>MyPath1</t>
+  </si>
+  <si>
+    <t>MyPath2</t>
+  </si>
+  <si>
+    <t>TEXTFILE</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
@@ -2169,6 +2197,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2254,11 +2283,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
@@ -2662,12 +2691,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>609</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="1"/>
       <c r="G2" s="5" t="s">
         <v>612</v>
@@ -2683,7 +2712,7 @@
       <c r="B3" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>607</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -5467,13 +5496,13 @@
       <c r="B162" s="2">
         <v>159</v>
       </c>
-      <c r="C162" s="9" t="s">
+      <c r="C162" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="D162" s="8" t="s">
+      <c r="D162" s="7" t="s">
         <v>609</v>
       </c>
-      <c r="E162" s="8" t="s">
+      <c r="E162" s="7" t="s">
         <v>702</v>
       </c>
       <c r="H162">
@@ -8242,8 +8271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D17882-7E2B-47E5-8D21-7E0595521524}">
   <dimension ref="B3:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8300,7 +8329,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="6">
         <v>43733</v>
       </c>
       <c r="C5" t="s">
@@ -8316,12 +8345,13 @@
         <v>3983</v>
       </c>
       <c r="H5">
-        <v>15</v>
+        <f>'Participants @Events'!E5</f>
+        <v>122</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="6">
         <v>43733</v>
       </c>
       <c r="K5" t="s">
@@ -8335,7 +8365,7 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="B6" s="6">
         <v>43024</v>
       </c>
       <c r="C6" t="s">
@@ -8351,12 +8381,13 @@
         <v>5906</v>
       </c>
       <c r="H6">
-        <v>51</v>
+        <f>'Participants @Events'!E6</f>
+        <v>47</v>
       </c>
       <c r="I6">
         <v>2</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="6">
         <v>43024</v>
       </c>
       <c r="K6" t="s">
@@ -8370,7 +8401,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="B7" s="6">
         <v>43078</v>
       </c>
       <c r="C7" t="s">
@@ -8386,12 +8417,13 @@
         <v>6331</v>
       </c>
       <c r="H7">
-        <v>131</v>
+        <f>'Participants @Events'!E7</f>
+        <v>20</v>
       </c>
       <c r="I7">
         <v>3</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="6">
         <v>43078</v>
       </c>
       <c r="K7" t="s">
@@ -8405,7 +8437,7 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="6">
         <v>42909</v>
       </c>
       <c r="C8" t="s">
@@ -8421,12 +8453,13 @@
         <v>126</v>
       </c>
       <c r="H8">
-        <v>132</v>
+        <f>'Participants @Events'!E8</f>
+        <v>126</v>
       </c>
       <c r="I8">
         <v>4</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="6">
         <v>42909</v>
       </c>
       <c r="K8" t="s">
@@ -8440,7 +8473,7 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="B9" s="6">
         <v>43737</v>
       </c>
       <c r="C9" t="s">
@@ -8456,12 +8489,13 @@
         <v>1490</v>
       </c>
       <c r="H9">
-        <v>95</v>
+        <f>'Participants @Events'!E9</f>
+        <v>73</v>
       </c>
       <c r="I9">
         <v>5</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="6">
         <v>43737</v>
       </c>
       <c r="K9" t="s">
@@ -8475,7 +8509,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="B10" s="6">
         <v>43692</v>
       </c>
       <c r="C10" t="s">
@@ -8491,12 +8525,13 @@
         <v>2620</v>
       </c>
       <c r="H10">
-        <v>16</v>
+        <f>'Participants @Events'!E10</f>
+        <v>52</v>
       </c>
       <c r="I10">
         <v>6</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="6">
         <v>43692</v>
       </c>
       <c r="K10" t="s">
@@ -8510,7 +8545,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="B11" s="6">
         <v>42896</v>
       </c>
       <c r="C11" t="s">
@@ -8526,12 +8561,13 @@
         <v>2424</v>
       </c>
       <c r="H11">
-        <v>91</v>
+        <f>'Participants @Events'!E11</f>
+        <v>10</v>
       </c>
       <c r="I11">
         <v>7</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="6">
         <v>42896</v>
       </c>
       <c r="K11" t="s">
@@ -8545,7 +8581,7 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="B12" s="6">
         <v>43177</v>
       </c>
       <c r="C12" t="s">
@@ -8561,12 +8597,13 @@
         <v>5894</v>
       </c>
       <c r="H12">
-        <v>156</v>
+        <f>'Participants @Events'!E12</f>
+        <v>158</v>
       </c>
       <c r="I12">
         <v>8</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="6">
         <v>43177</v>
       </c>
       <c r="K12" t="s">
@@ -8580,7 +8617,7 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="B13" s="6">
         <v>43165</v>
       </c>
       <c r="C13" t="s">
@@ -8596,12 +8633,13 @@
         <v>4290</v>
       </c>
       <c r="H13">
-        <v>50</v>
+        <f>'Participants @Events'!E13</f>
+        <v>148</v>
       </c>
       <c r="I13">
         <v>9</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="6">
         <v>43165</v>
       </c>
       <c r="K13" t="s">
@@ -8615,7 +8653,7 @@
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="B14" s="6">
         <v>43109</v>
       </c>
       <c r="C14" t="s">
@@ -8631,12 +8669,13 @@
         <v>660</v>
       </c>
       <c r="H14">
-        <v>149</v>
+        <f>'Participants @Events'!E14</f>
+        <v>38</v>
       </c>
       <c r="I14">
         <v>10</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="6">
         <v>43109</v>
       </c>
       <c r="K14" t="s">
@@ -8650,7 +8689,7 @@
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="B15" s="6">
         <v>43687</v>
       </c>
       <c r="C15" t="s">
@@ -8666,12 +8705,13 @@
         <v>6446</v>
       </c>
       <c r="H15">
-        <v>32</v>
+        <f>'Participants @Events'!E15</f>
+        <v>27</v>
       </c>
       <c r="I15">
         <v>11</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="6">
         <v>43687</v>
       </c>
       <c r="K15" t="s">
@@ -8685,7 +8725,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="B16" s="6">
         <v>43534</v>
       </c>
       <c r="C16" t="s">
@@ -8701,12 +8741,13 @@
         <v>664</v>
       </c>
       <c r="H16">
-        <v>129</v>
+        <f>'Participants @Events'!E16</f>
+        <v>87</v>
       </c>
       <c r="I16">
         <v>12</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="6">
         <v>43534</v>
       </c>
       <c r="K16" t="s">
@@ -8720,7 +8761,7 @@
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="B17" s="6">
         <v>43155</v>
       </c>
       <c r="C17" t="s">
@@ -8736,12 +8777,13 @@
         <v>4330</v>
       </c>
       <c r="H17">
-        <v>66</v>
+        <f>'Participants @Events'!E17</f>
+        <v>20</v>
       </c>
       <c r="I17">
         <v>13</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="6">
         <v>43155</v>
       </c>
       <c r="K17" t="s">
@@ -8755,7 +8797,7 @@
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="B18" s="6">
         <v>43706</v>
       </c>
       <c r="C18" t="s">
@@ -8771,12 +8813,13 @@
         <v>669</v>
       </c>
       <c r="H18">
-        <v>102</v>
+        <f>'Participants @Events'!E18</f>
+        <v>83</v>
       </c>
       <c r="I18">
         <v>14</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="6">
         <v>43706</v>
       </c>
       <c r="K18" t="s">
@@ -8790,7 +8833,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="B19" s="6">
         <v>43692</v>
       </c>
       <c r="C19" t="s">
@@ -8806,12 +8849,13 @@
         <v>6722</v>
       </c>
       <c r="H19">
-        <v>96</v>
+        <f>'Participants @Events'!E19</f>
+        <v>128</v>
       </c>
       <c r="I19">
         <v>15</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="6">
         <v>43692</v>
       </c>
       <c r="K19" t="s">
@@ -8825,7 +8869,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="B20" s="6">
         <v>43404</v>
       </c>
       <c r="C20" t="s">
@@ -8841,12 +8885,13 @@
         <v>3137</v>
       </c>
       <c r="H20">
-        <v>39</v>
+        <f>'Participants @Events'!E20</f>
+        <v>27</v>
       </c>
       <c r="I20">
         <v>16</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="6">
         <v>43404</v>
       </c>
       <c r="K20" t="s">
@@ -8857,6 +8902,108 @@
       </c>
       <c r="M20" t="s">
         <v>695</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4943BD2-34E8-4344-A992-7ECCD800397B}">
+  <dimension ref="B3:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>703</v>
+      </c>
+      <c r="F3" t="s">
+        <v>704</v>
+      </c>
+      <c r="I3" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>605</v>
+      </c>
+      <c r="C4" t="s">
+        <v>672</v>
+      </c>
+      <c r="F4" t="s">
+        <v>605</v>
+      </c>
+      <c r="G4" t="s">
+        <v>705</v>
+      </c>
+      <c r="I4" t="s">
+        <v>605</v>
+      </c>
+      <c r="J4" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>706</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>707</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>